<commit_message>
Feat: check_rev, main_menu, main_menu(1-4, 1-5), theater.xlsx 수정본
</commit_message>
<xml_diff>
--- a/theater/theater.xlsx
+++ b/theater/theater.xlsx
@@ -450,10 +450,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -464,7 +464,7 @@
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3">
@@ -502,7 +502,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -540,7 +540,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9">
@@ -578,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">

</xml_diff>